<commit_message>
added runtime exception for checking the version
</commit_message>
<xml_diff>
--- a/io-table-xlsx/testWrite.xlsx
+++ b/io-table-xlsx/testWrite.xlsx
@@ -6,7 +6,7 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="data" r:id="rId3" sheetId="1"/>
+    <sheet name="ooo" r:id="rId3" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
@@ -15,7 +15,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
-    <author>io.table</author>
+    <author>IZARMobile</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="1">
@@ -155,7 +155,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="n" s="2">
-        <v>43180.40852320602</v>
+        <v>43180.41794226852</v>
       </c>
     </row>
     <row r="4">

</xml_diff>